<commit_message>
Added UI and began bug fixing
</commit_message>
<xml_diff>
--- a/Output/ChaoticThunder0.xlsx
+++ b/Output/ChaoticThunder0.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,7 +447,7 @@
           <t>Red Team</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Blue Team</t>
         </is>
@@ -459,83 +459,143 @@
           <t>12/22/2022, 21:55:59</t>
         </is>
       </c>
-      <c r="B2" s="3" t="n"/>
+      <c r="C2" s="3" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
-          <t>runes</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="n"/>
-      <c r="C3" s="4" t="inlineStr">
-        <is>
-          <t>runes</t>
+          <t>summonerName</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>championName</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>summonerName</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>championName</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Conquerorand Second Wind</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="n"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Lethal Tempoand Biscuit Delivery</t>
+          <t>ToastifiedToast</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Gwen</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Tosh Gaming</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Jax</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Dark Harvestand Celerity</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="n"/>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Aftershockand Triumph</t>
+          <t>kwondii</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Nunu</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>ChaoticThunder0</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Rammus</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Electrocuteand Manaflow Band</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="n"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Lethal Tempoand Bone Plating</t>
+          <t>cocollona</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Anivia</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="n"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>ojded</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Yasuo</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>First Strikeand Manaflow Band</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="n"/>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Lethal Tempoand Biscuit Delivery</t>
+          <t>ComeHereDumBoi</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ezreal</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>novaunreprising</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Jinx</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Summon Aeryand Bone Plating</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="n"/>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>First Strikeand Manaflow Band</t>
+          <t>vin00000</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Seraphine</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="n"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Speedojoe</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Xerath</t>
         </is>
       </c>
     </row>
@@ -545,7 +605,7 @@
           <t>Red Team</t>
         </is>
       </c>
-      <c r="C9" s="1" t="inlineStr">
+      <c r="D9" s="1" t="inlineStr">
         <is>
           <t>Blue Team</t>
         </is>
@@ -557,83 +617,143 @@
           <t>12/21/2022, 22:42:08</t>
         </is>
       </c>
-      <c r="B10" s="3" t="n"/>
+      <c r="C10" s="3" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>runes</t>
-        </is>
-      </c>
-      <c r="B11" s="3" t="n"/>
-      <c r="C11" s="4" t="inlineStr">
-        <is>
-          <t>runes</t>
+          <t>summonerName</t>
+        </is>
+      </c>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>championName</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="n"/>
+      <c r="D11" s="4" t="inlineStr">
+        <is>
+          <t>summonerName</t>
+        </is>
+      </c>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
+          <t>championName</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Press the Attackand Bone Plating</t>
-        </is>
-      </c>
-      <c r="B12" s="3" t="n"/>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Grasp of the Undyingand Cheap Shot</t>
+          <t>Reminessance</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Teemo</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="n"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>GrumpyGarbage</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Shen</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Conquerorand Magical Footwear</t>
-        </is>
-      </c>
-      <c r="B13" s="3" t="n"/>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Conquerorand Conditioning</t>
+          <t>TheeBlackLegacy</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Kayn</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="n"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>ChaoticThunder0</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Mordekaiser</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Lethal Tempoand Biscuit Delivery</t>
-        </is>
-      </c>
-      <c r="B14" s="3" t="n"/>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Conquerorand Second Wind</t>
+          <t>Zatnoss</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Irelia</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="n"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>ben jk</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Syndra</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Press the Attackand Magical Footwear</t>
-        </is>
-      </c>
-      <c r="B15" s="3" t="n"/>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Lethal Tempoand Magical Footwear</t>
+          <t>ueatdirt</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>MissFortune</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="n"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>OmniWaffleGod73</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Ashe</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Arcane Cometand Biscuit Delivery</t>
-        </is>
-      </c>
-      <c r="B16" s="3" t="n"/>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Electrocuteand Coup de Grace</t>
+          <t>svckit</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Lux</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="n"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Bubblesf</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Anivia</t>
         </is>
       </c>
     </row>
@@ -643,7 +763,7 @@
           <t>Red Team</t>
         </is>
       </c>
-      <c r="C17" s="1" t="inlineStr">
+      <c r="D17" s="1" t="inlineStr">
         <is>
           <t>Blue Team</t>
         </is>
@@ -655,83 +775,143 @@
           <t>12/21/2022, 22:01:25</t>
         </is>
       </c>
-      <c r="B18" s="3" t="n"/>
+      <c r="C18" s="3" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
         <is>
-          <t>runes</t>
-        </is>
-      </c>
-      <c r="B19" s="3" t="n"/>
-      <c r="C19" s="4" t="inlineStr">
-        <is>
-          <t>runes</t>
+          <t>summonerName</t>
+        </is>
+      </c>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t>championName</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="n"/>
+      <c r="D19" s="4" t="inlineStr">
+        <is>
+          <t>summonerName</t>
+        </is>
+      </c>
+      <c r="E19" s="4" t="inlineStr">
+        <is>
+          <t>championName</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Conquerorand Revitalize</t>
-        </is>
-      </c>
-      <c r="B20" s="3" t="n"/>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Conquerorand Second Wind</t>
+          <t>BWstrikesback</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>MonkeyKing</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="n"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>3xtraChr0m0s0me</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Mordekaiser</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Hail of Bladesand Celerity</t>
-        </is>
-      </c>
-      <c r="B21" s="3" t="n"/>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Conquerorand Conditioning</t>
+          <t>ChaoticThunder0</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Udyr</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="n"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>apaid</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Sett</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>First Strikeand Manaflow Band</t>
-        </is>
-      </c>
-      <c r="B22" s="3" t="n"/>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Electrocuteand Triumph</t>
+          <t>Becker1099</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Zoe</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="n"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>snail chloride</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Talon</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Electrocuteand Manaflow Band</t>
-        </is>
-      </c>
-      <c r="B23" s="3" t="n"/>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Lethal Tempoand Absolute Focus</t>
+          <t>OmniWaffleGod73</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Veigar</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="n"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>sushiguyalex</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Caitlyn</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Conquerorand Second Wind</t>
-        </is>
-      </c>
-      <c r="B24" s="3" t="n"/>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Electrocuteand Manaflow Band</t>
+          <t>Bubblesf</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Swain</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="n"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Fartingzest</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Vex</t>
         </is>
       </c>
     </row>
@@ -741,7 +921,7 @@
           <t>Red Team</t>
         </is>
       </c>
-      <c r="C25" s="1" t="inlineStr">
+      <c r="D25" s="1" t="inlineStr">
         <is>
           <t>Blue Team</t>
         </is>
@@ -753,83 +933,143 @@
           <t>12/21/2022, 21:00:19</t>
         </is>
       </c>
-      <c r="B26" s="3" t="n"/>
+      <c r="C26" s="3" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="4" t="inlineStr">
         <is>
-          <t>runes</t>
-        </is>
-      </c>
-      <c r="B27" s="3" t="n"/>
-      <c r="C27" s="4" t="inlineStr">
-        <is>
-          <t>runes</t>
+          <t>summonerName</t>
+        </is>
+      </c>
+      <c r="B27" s="4" t="inlineStr">
+        <is>
+          <t>championName</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="n"/>
+      <c r="D27" s="4" t="inlineStr">
+        <is>
+          <t>summonerName</t>
+        </is>
+      </c>
+      <c r="E27" s="4" t="inlineStr">
+        <is>
+          <t>championName</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Arcane Cometand Perfect Timing</t>
-        </is>
-      </c>
-      <c r="B28" s="3" t="n"/>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Grasp of the Undyingand Legend: Tenacity</t>
+          <t>NameYourPoisonPl</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Heimerdinger</t>
+        </is>
+      </c>
+      <c r="C28" s="3" t="n"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Wild Oblivion</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Chogath</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Hail of Bladesand Celerity</t>
-        </is>
-      </c>
-      <c r="B29" s="3" t="n"/>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Aftershockand Cheap Shot</t>
+          <t>ChaoticThunder0</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Udyr</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="n"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>CM876</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Sejuani</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>First Strikeand Manaflow Band</t>
-        </is>
-      </c>
-      <c r="B30" s="3" t="n"/>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Electrocuteand Manaflow Band</t>
+          <t>TexxxasSausage</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Syndra</t>
+        </is>
+      </c>
+      <c r="C30" s="3" t="n"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Owlz03</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Ahri</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Conquerorand Taste of Blood</t>
-        </is>
-      </c>
-      <c r="B31" s="3" t="n"/>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Lethal Tempoand Taste of Blood</t>
+          <t>Sex With Haru</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Samira</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="n"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Hoerizontal</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Varus</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>First Strikeand Absolute Focus</t>
-        </is>
-      </c>
-      <c r="B32" s="3" t="n"/>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Press the Attackand Cheap Shot</t>
+          <t>cheesytitz</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Xerath</t>
+        </is>
+      </c>
+      <c r="C32" s="3" t="n"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>OVOFrostbyte707</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Pantheon</t>
         </is>
       </c>
     </row>
@@ -839,7 +1079,7 @@
           <t>Red Team</t>
         </is>
       </c>
-      <c r="C33" s="1" t="inlineStr">
+      <c r="D33" s="1" t="inlineStr">
         <is>
           <t>Blue Team</t>
         </is>
@@ -851,83 +1091,143 @@
           <t>12/20/2022, 23:53:55</t>
         </is>
       </c>
-      <c r="B34" s="3" t="n"/>
+      <c r="C34" s="3" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="4" t="inlineStr">
         <is>
-          <t>runes</t>
-        </is>
-      </c>
-      <c r="B35" s="3" t="n"/>
-      <c r="C35" s="4" t="inlineStr">
-        <is>
-          <t>runes</t>
+          <t>summonerName</t>
+        </is>
+      </c>
+      <c r="B35" s="4" t="inlineStr">
+        <is>
+          <t>championName</t>
+        </is>
+      </c>
+      <c r="C35" s="3" t="n"/>
+      <c r="D35" s="4" t="inlineStr">
+        <is>
+          <t>summonerName</t>
+        </is>
+      </c>
+      <c r="E35" s="4" t="inlineStr">
+        <is>
+          <t>championName</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Electrocuteand Absolute Focus</t>
-        </is>
-      </c>
-      <c r="B36" s="3" t="n"/>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Grasp of the Undyingand Manaflow Band</t>
+          <t>W0ckhardtWarri0r</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Kennen</t>
+        </is>
+      </c>
+      <c r="C36" s="3" t="n"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>kymchee</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Fiora</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Conquerorand Conditioning</t>
-        </is>
-      </c>
-      <c r="B37" s="3" t="n"/>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Conquerorand Revitalize</t>
+          <t>ChaoticThunder0</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Volibear</t>
+        </is>
+      </c>
+      <c r="C37" s="3" t="n"/>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>LimeDinosaur</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Warwick</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Electrocuteand Triumph</t>
-        </is>
-      </c>
-      <c r="B38" s="3" t="n"/>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Dark Harvestand Cosmic Insight</t>
+          <t>FaZeWoJo</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Katarina</t>
+        </is>
+      </c>
+      <c r="C38" s="3" t="n"/>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>l0velymoch1</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Teemo</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Fleet Footworkand Absolute Focus</t>
-        </is>
-      </c>
-      <c r="B39" s="3" t="n"/>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Lethal Tempoand Absolute Focus</t>
+          <t>Zek3PlayS</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Caitlyn</t>
+        </is>
+      </c>
+      <c r="C39" s="3" t="n"/>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>farisfreek</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Jinx</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Glacial Augmentand Bone Plating</t>
-        </is>
-      </c>
-      <c r="B40" s="3" t="n"/>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Summon Aeryand Biscuit Delivery</t>
+          <t>KMJ1000</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Thresh</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="n"/>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>remierat</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Seraphine</t>
         </is>
       </c>
     </row>
@@ -937,7 +1237,7 @@
           <t>Red Team</t>
         </is>
       </c>
-      <c r="C41" s="1" t="inlineStr">
+      <c r="D41" s="1" t="inlineStr">
         <is>
           <t>Blue Team</t>
         </is>
@@ -949,83 +1249,143 @@
           <t>12/20/2022, 23:26:14</t>
         </is>
       </c>
-      <c r="B42" s="3" t="n"/>
+      <c r="C42" s="3" t="n"/>
     </row>
     <row r="43">
       <c r="A43" s="4" t="inlineStr">
         <is>
-          <t>runes</t>
-        </is>
-      </c>
-      <c r="B43" s="3" t="n"/>
-      <c r="C43" s="4" t="inlineStr">
-        <is>
-          <t>runes</t>
+          <t>summonerName</t>
+        </is>
+      </c>
+      <c r="B43" s="4" t="inlineStr">
+        <is>
+          <t>championName</t>
+        </is>
+      </c>
+      <c r="C43" s="3" t="n"/>
+      <c r="D43" s="4" t="inlineStr">
+        <is>
+          <t>summonerName</t>
+        </is>
+      </c>
+      <c r="E43" s="4" t="inlineStr">
+        <is>
+          <t>championName</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Fleet Footworkand Second Wind</t>
-        </is>
-      </c>
-      <c r="B44" s="3" t="n"/>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Conquerorand Bone Plating</t>
+          <t>joking2no</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Nasus</t>
+        </is>
+      </c>
+      <c r="C44" s="3" t="n"/>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>AKAVapeon</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Illaoi</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Lethal Tempoand Celerity</t>
-        </is>
-      </c>
-      <c r="B45" s="3" t="n"/>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Conquerorand Nimbus Cloak</t>
+          <t>FlashDr1ppp</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Warwick</t>
+        </is>
+      </c>
+      <c r="C45" s="3" t="n"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>ChaoticThunder0</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Hecarim</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Summon Aeryand Demolish</t>
-        </is>
-      </c>
-      <c r="B46" s="3" t="n"/>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Electrocuteand Absolute Focus</t>
+          <t>The Seamen Demon</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Diana</t>
+        </is>
+      </c>
+      <c r="C46" s="3" t="n"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>TheNobleInc</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Talon</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Lethal Tempoand Biscuit Delivery</t>
-        </is>
-      </c>
-      <c r="B47" s="3" t="n"/>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Lethal Tempoand Magical Footwear</t>
+          <t>soggycerealtf</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Ashe</t>
+        </is>
+      </c>
+      <c r="C47" s="3" t="n"/>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>P0niesDaughter</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>MissFortune</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Guardianand Approach Velocity</t>
-        </is>
-      </c>
-      <c r="B48" s="3" t="n"/>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Arcane Cometand Cheap Shot</t>
+          <t>Błender</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Braum</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="n"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>OG Bruniik</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Lux</t>
         </is>
       </c>
     </row>
@@ -1035,7 +1395,7 @@
           <t>Red Team</t>
         </is>
       </c>
-      <c r="C49" s="1" t="inlineStr">
+      <c r="D49" s="1" t="inlineStr">
         <is>
           <t>Blue Team</t>
         </is>
@@ -1047,83 +1407,143 @@
           <t>12/19/2022, 23:11:39</t>
         </is>
       </c>
-      <c r="B50" s="3" t="n"/>
+      <c r="C50" s="3" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="4" t="inlineStr">
         <is>
-          <t>runes</t>
-        </is>
-      </c>
-      <c r="B51" s="3" t="n"/>
-      <c r="C51" s="4" t="inlineStr">
-        <is>
-          <t>runes</t>
+          <t>summonerName</t>
+        </is>
+      </c>
+      <c r="B51" s="4" t="inlineStr">
+        <is>
+          <t>championName</t>
+        </is>
+      </c>
+      <c r="C51" s="3" t="n"/>
+      <c r="D51" s="4" t="inlineStr">
+        <is>
+          <t>summonerName</t>
+        </is>
+      </c>
+      <c r="E51" s="4" t="inlineStr">
+        <is>
+          <t>championName</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Conquerorand Overgrowth</t>
-        </is>
-      </c>
-      <c r="B52" s="3" t="n"/>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Conquerorand Revitalize</t>
+          <t>ThermalSquash</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Garen</t>
+        </is>
+      </c>
+      <c r="C52" s="3" t="n"/>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>bdht06</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Mordekaiser</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Conquerorand Nimbus Cloak</t>
-        </is>
-      </c>
-      <c r="B53" s="3" t="n"/>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Conquerorand Magical Footwear</t>
+          <t>ChaoticThunder0</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Hecarim</t>
+        </is>
+      </c>
+      <c r="C53" s="3" t="n"/>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Aklaintac</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>LeeSin</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>First Strikeand Transcendence</t>
-        </is>
-      </c>
-      <c r="B54" s="3" t="n"/>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Lethal Tempoand Second Wind</t>
+          <t>Bonecollector584</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Shyvana</t>
+        </is>
+      </c>
+      <c r="C54" s="3" t="n"/>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Shiroishi25</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Yone</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Press the Attackand Magical Footwear</t>
-        </is>
-      </c>
-      <c r="B55" s="3" t="n"/>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Press the Attackand Taste of Blood</t>
+          <t>SharpDressedLad</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>MissFortune</t>
+        </is>
+      </c>
+      <c r="C55" s="3" t="n"/>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>ExpelliarmusEX</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Vayne</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Arcane Cometand Ultimate Hunter</t>
-        </is>
-      </c>
-      <c r="B56" s="3" t="n"/>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Summon Aeryand Biscuit Delivery</t>
+          <t>Yalta808</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Lux</t>
+        </is>
+      </c>
+      <c r="C56" s="3" t="n"/>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>x Taylor Swift x</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Seraphine</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1553,7 @@
           <t>Red Team</t>
         </is>
       </c>
-      <c r="C57" s="1" t="inlineStr">
+      <c r="D57" s="1" t="inlineStr">
         <is>
           <t>Blue Team</t>
         </is>
@@ -1145,112 +1565,172 @@
           <t>12/19/2022, 22:36:48</t>
         </is>
       </c>
-      <c r="B58" s="3" t="n"/>
+      <c r="C58" s="3" t="n"/>
     </row>
     <row r="59">
       <c r="A59" s="4" t="inlineStr">
         <is>
-          <t>runes</t>
-        </is>
-      </c>
-      <c r="B59" s="3" t="n"/>
-      <c r="C59" s="4" t="inlineStr">
-        <is>
-          <t>runes</t>
+          <t>summonerName</t>
+        </is>
+      </c>
+      <c r="B59" s="4" t="inlineStr">
+        <is>
+          <t>championName</t>
+        </is>
+      </c>
+      <c r="C59" s="3" t="n"/>
+      <c r="D59" s="4" t="inlineStr">
+        <is>
+          <t>summonerName</t>
+        </is>
+      </c>
+      <c r="E59" s="4" t="inlineStr">
+        <is>
+          <t>championName</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Summon Aeryand Bone Plating</t>
-        </is>
-      </c>
-      <c r="B60" s="3" t="n"/>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Aftershockand Biscuit Delivery</t>
+          <t>Ritzsu</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Renata</t>
+        </is>
+      </c>
+      <c r="C60" s="3" t="n"/>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>SLG Poopies</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Blitzcrank</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Hail of Bladesand Legend: Bloodline</t>
-        </is>
-      </c>
-      <c r="B61" s="3" t="n"/>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>Lethal Tempoand Absolute Focus</t>
+          <t>shadowbunner</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Tristana</t>
+        </is>
+      </c>
+      <c r="C61" s="3" t="n"/>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Soliditaryy</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Caitlyn</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Press the Attackand Conditioning</t>
-        </is>
-      </c>
-      <c r="B62" s="3" t="n"/>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>Grasp of the Undyingand Manaflow Band</t>
+          <t>Sickgamer69</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Urgot</t>
+        </is>
+      </c>
+      <c r="C62" s="3" t="n"/>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>thiccsuccdank</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Chogath</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Hail of Bladesand Absolute Focus</t>
-        </is>
-      </c>
-      <c r="B63" s="3" t="n"/>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>Electrocuteand Magical Footwear</t>
+          <t>thelegend592</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Varus</t>
+        </is>
+      </c>
+      <c r="C63" s="3" t="n"/>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Wanchu</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Rengar</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Conquerorand Conditioning</t>
-        </is>
-      </c>
-      <c r="B64" s="3" t="n"/>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Arcane Cometand Cheap Shot</t>
+          <t>ChaoticThunder0</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Mordekaiser</t>
+        </is>
+      </c>
+      <c r="C64" s="3" t="n"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>SLG Sarahkiins</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Lux</t>
         </is>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A1"/>
-    <mergeCell ref="C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9"/>
-    <mergeCell ref="C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A17"/>
-    <mergeCell ref="C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A25"/>
-    <mergeCell ref="C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A33"/>
-    <mergeCell ref="C33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A41"/>
-    <mergeCell ref="C41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A49"/>
-    <mergeCell ref="C49"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A57"/>
-    <mergeCell ref="C57"/>
-    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="A58:E58"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>